<commit_message>
Updated to version 2.4
</commit_message>
<xml_diff>
--- a/walter-feels/production/walter-feels-bom.xlsx
+++ b/walter-feels/production/walter-feels-bom.xlsx
@@ -111,7 +111,7 @@
     <t xml:space="preserve">100pF ±5%, 50V, C0G, 0603 MLCC</t>
   </si>
   <si>
-    <t xml:space="preserve">C5, C8, C10, C11, C18, C21, C24, C62, C70, C77, C79 </t>
+    <t xml:space="preserve">C5, C8, C10, C11, C18, C21, C24, C62, C70, C79 </t>
   </si>
   <si>
     <t xml:space="preserve">10µF</t>
@@ -248,7 +248,7 @@
     <t xml:space="preserve">33nF ±10%, 50V, X7R, 0603 MLCC</t>
   </si>
   <si>
-    <t xml:space="preserve">C60</t>
+    <t xml:space="preserve">C60, C77</t>
   </si>
   <si>
     <t xml:space="preserve">4.7μF</t>
@@ -1346,7 +1346,7 @@
   <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1359,7 +1359,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="8" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16380" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16380" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1468,7 +1468,7 @@
         <v>21</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>10</v>
@@ -1721,7 +1721,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>10</v>

</xml_diff>